<commit_message>
after dealing with exeptions
</commit_message>
<xml_diff>
--- a/IMDB.xlsx
+++ b/IMDB.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D251"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,11 @@
           <t>rate</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>popularity</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +469,11 @@
           <t>9.2</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +496,11 @@
           <t>9.2</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,6 +523,11 @@
           <t>9.0</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -530,6 +550,11 @@
           <t>9.0</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -552,6 +577,11 @@
           <t>8.9</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>394</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -574,6 +604,11 @@
           <t>8.9</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>217</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -596,6 +631,11 @@
           <t>8.9</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>371</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -618,6 +658,11 @@
           <t>8.9</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -640,6 +685,11 @@
           <t>8.8</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>182</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -662,6 +712,11 @@
           <t>8.8</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>561</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -684,6 +739,11 @@
           <t>8.8</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -706,6 +766,11 @@
           <t>8.7</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -728,6 +793,11 @@
           <t>8.7</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>119</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -750,6 +820,11 @@
           <t>8.7</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -772,6 +847,11 @@
           <t>8.7</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>222</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -794,6 +874,11 @@
           <t>8.7</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>326</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -816,6 +901,11 @@
           <t>8.7</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>142</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -838,6 +928,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>505</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -860,6 +955,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -882,6 +982,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1,521</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -904,6 +1009,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1,501</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -926,6 +1036,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>232</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -948,6 +1063,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>602</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -970,6 +1090,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -992,6 +1117,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1014,6 +1144,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1036,6 +1171,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1058,6 +1198,11 @@
           <t>8.6</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1080,6 +1225,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>549</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1102,6 +1252,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1124,6 +1279,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>513</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1146,6 +1306,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>721</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1168,6 +1333,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>718</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1190,6 +1360,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>158</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1212,6 +1387,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1234,6 +1414,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>281</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1256,6 +1441,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>287</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1278,6 +1468,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1300,6 +1495,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>462</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1322,6 +1522,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>167</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1344,6 +1549,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>352</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1366,6 +1576,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>1,007</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1388,6 +1603,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1410,6 +1630,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1432,6 +1657,11 @@
           <t>8.5</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1454,6 +1684,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1476,6 +1711,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>3,174</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1498,6 +1738,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>1,406</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1520,6 +1765,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>1,382</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1542,6 +1792,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1,624</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1564,6 +1819,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1586,6 +1846,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1608,6 +1873,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2,135</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1630,6 +1900,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>608</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1652,6 +1927,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>231</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1674,6 +1954,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>370</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1696,6 +1981,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1718,6 +2008,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>863</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1740,6 +2035,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>1,196</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1762,6 +2062,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2,538</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1784,6 +2089,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3,505</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1806,6 +2116,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>332</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1828,6 +2143,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>4,457</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1850,6 +2170,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>3,383</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1872,6 +2197,11 @@
           <t>8.4</t>
         </is>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1894,6 +2224,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>271</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1916,6 +2251,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>322</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1938,6 +2278,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>1,063</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1960,6 +2305,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>318</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1982,6 +2332,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>296</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2004,6 +2359,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>428</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2026,6 +2386,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>161</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2048,6 +2413,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>1,105</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2070,6 +2440,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>598</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2092,6 +2467,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>163</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2114,6 +2494,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>734</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2136,6 +2521,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>1,658</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2158,6 +2548,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>169</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2180,6 +2575,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>1,603</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2202,6 +2602,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2224,6 +2629,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2246,6 +2656,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>389</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2268,6 +2683,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2290,6 +2710,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2312,6 +2737,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>980</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2334,6 +2764,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2,094</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2356,6 +2791,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>987</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2378,6 +2818,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2400,6 +2845,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>668</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2422,6 +2872,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>469</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2444,6 +2899,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>621</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2466,6 +2926,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2488,6 +2953,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>1,565</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2510,6 +2980,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>1,863</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2532,6 +3007,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>1,562</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2554,6 +3034,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>593</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2576,6 +3061,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2,741</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2598,6 +3088,11 @@
           <t>8.3</t>
         </is>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>1,138</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2620,6 +3115,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2,109</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2642,6 +3142,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>1,098</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2664,6 +3169,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>383</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2686,6 +3196,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>962</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2708,6 +3223,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>346</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2730,6 +3250,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2,847</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2752,6 +3277,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2,765</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2774,6 +3304,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>366</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2796,6 +3331,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2818,6 +3358,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>1,290</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2840,6 +3385,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>1,632</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2862,6 +3412,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2884,6 +3439,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>915</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2906,6 +3466,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>864</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2928,6 +3493,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2950,6 +3520,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>527</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2972,6 +3547,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2,592</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2994,6 +3574,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>3,042</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3016,6 +3601,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>520</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3038,6 +3628,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>562</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3060,6 +3655,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3082,6 +3682,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>883</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3104,6 +3709,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3126,6 +3736,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3148,6 +3763,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3170,6 +3790,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>3,928</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3192,6 +3817,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>1,222</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3214,6 +3844,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>3,262</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3236,6 +3871,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>470</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3258,6 +3898,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>3,586</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3280,6 +3925,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3302,6 +3952,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>1,505</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3324,6 +3979,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>667</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3346,6 +4006,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>4,007</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3368,6 +4033,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>642</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3390,6 +4060,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3412,6 +4087,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>3,300</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3434,6 +4114,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3456,6 +4141,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>1,024</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3478,6 +4168,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>3,033</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3500,6 +4195,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>557</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3522,6 +4222,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>927</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3544,6 +4249,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>452</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3566,6 +4276,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>516</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3588,6 +4303,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>573</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3610,6 +4330,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>1,408</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3632,6 +4357,11 @@
           <t>8.2</t>
         </is>
       </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3654,6 +4384,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -3676,6 +4411,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3698,6 +4438,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>341</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -3720,6 +4465,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -3742,6 +4492,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>2,410</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3764,6 +4519,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3786,6 +4546,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>566</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3808,6 +4573,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>304</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3830,6 +4600,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>686</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3852,6 +4627,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>2,536</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3874,6 +4654,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>1,857</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3896,6 +4681,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>397</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3918,6 +4708,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>1,164</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3940,6 +4735,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>865</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3962,6 +4762,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -3984,6 +4789,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>731</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -4006,6 +4816,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>1,006</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -4028,6 +4843,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>3,026</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -4050,6 +4870,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>2,289</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -4059,17 +4884,22 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Hauru no ugoku shiro</t>
+          <t>The Bridge on the River Kwai</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>1957</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
           <t>8.1</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>2,582</t>
         </is>
       </c>
     </row>
@@ -4081,17 +4911,22 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>The Bridge on the River Kwai</t>
+          <t>Hauru no ugoku shiro</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>1957</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
           <t>8.1</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>778</t>
         </is>
       </c>
     </row>
@@ -4116,6 +4951,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>885</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -4138,6 +4978,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>627</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -4160,6 +5005,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>1,431</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -4182,6 +5032,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>898</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -4204,6 +5059,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>579</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -4226,6 +5086,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>269</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -4248,6 +5113,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>2,158</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -4270,6 +5140,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>973</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -4292,6 +5167,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -4314,6 +5194,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>235</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -4336,6 +5221,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>568</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4358,6 +5248,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>2,954</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4380,6 +5275,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>4,312</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4402,6 +5302,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -4424,6 +5329,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>2,395</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -4446,6 +5356,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -4468,6 +5383,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>4,266</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4490,6 +5410,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -4512,6 +5437,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>305</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4534,6 +5464,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>743</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4556,6 +5491,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>553</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4578,6 +5518,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>974</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4600,6 +5545,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>2,450</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4622,6 +5572,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>171</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4644,6 +5599,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4666,6 +5626,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4688,6 +5653,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>2,126</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4710,6 +5680,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4732,6 +5707,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>1,075</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4754,6 +5734,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>893</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -4776,6 +5761,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>3,940</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -4798,6 +5788,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>336</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -4820,6 +5815,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>3,152</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -4842,6 +5842,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>2,627</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -4864,6 +5869,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>414</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -4886,6 +5896,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>213</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -4908,6 +5923,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>1,045</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -4930,6 +5950,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>4,626</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -4952,6 +5977,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>670</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -4974,6 +6004,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -4996,6 +6031,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -5018,6 +6058,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>3,638</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -5040,6 +6085,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -5062,6 +6112,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -5084,6 +6139,11 @@
           <t>8.1</t>
         </is>
       </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -5106,6 +6166,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>1,005</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -5128,6 +6193,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>846</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -5150,6 +6220,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>289</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -5172,6 +6247,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -5194,6 +6274,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>431</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -5216,6 +6301,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>1,035</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -5238,6 +6328,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>804</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -5260,6 +6355,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>267</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -5282,6 +6382,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>3,414</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -5304,6 +6409,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>445</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -5326,6 +6436,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>620</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -5348,6 +6463,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>515</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -5370,6 +6490,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>1,317</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -5392,6 +6517,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>1,821</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -5414,6 +6544,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>523</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -5436,6 +6571,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>3,617</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -5458,6 +6598,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>508</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -5480,6 +6625,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -5502,6 +6652,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>3,315</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -5524,6 +6679,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -5546,6 +6706,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -5568,6 +6733,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>2,482</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -5590,6 +6760,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>2,719</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -5612,6 +6787,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>3,468</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -5634,6 +6814,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -5656,6 +6841,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>2,651</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -5678,6 +6868,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -5700,6 +6895,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>3,050</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -5722,6 +6922,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -5744,6 +6949,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>2,532</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -5766,6 +6976,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>NotFound</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -5788,6 +7003,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>204</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -5810,6 +7030,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>4,519</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -5832,6 +7057,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>499</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -5854,6 +7084,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>1,034</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -5876,6 +7111,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>3,063</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -5898,6 +7138,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>2,683</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -5920,6 +7165,11 @@
           <t>8.0</t>
         </is>
       </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>761</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -5940,6 +7190,11 @@
       <c r="D251" t="inlineStr">
         <is>
           <t>8.0</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>1,145</t>
         </is>
       </c>
     </row>

</xml_diff>